<commit_message>
Remove form_id from remaining forms
</commit_message>
<xml_diff>
--- a/case-id/forms/app/case_event.xlsx
+++ b/case-id/forms/app/case_event.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -118,9 +118,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique ID that identifies this form to tools that use it. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. 
-For example: bench_inventory_2021
-You can change the form_title as much as you would like but if you change the form_id, it will be considered a different form definition.</t>
+          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
+By default, this template uses a formula to create a date-based version that will update automatically.</t>
         </r>
       </text>
     </comment>
@@ -132,24 +131,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
-By default, this template uses a formula to create a date-based version that will update automatically.</t>
+          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
         </r>
       </text>
     </comment>
     <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -192,9 +178,6 @@
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">version</t>
   </si>
   <si>
@@ -205,9 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">Add Case Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_event</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -699,7 +679,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -739,7 +719,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A28:D10000 A27:B27 D2:D27 A2:C26">
+  <conditionalFormatting sqref="A2:D10000">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -761,31 +741,9 @@
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26">
+  <conditionalFormatting sqref="C2:C10000">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A27="begin_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A27="end_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A27="begin_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A27="end_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -814,18 +772,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,26 +798,20 @@
       <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20260114092650</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="6" t="str">
-        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213155202</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>